<commit_message>
added loading excel from buffer, removing path so its compatible with browser
</commit_message>
<xml_diff>
--- a/test_data/additional/additional-ro-crate-metadata.xlsx
+++ b/test_data/additional/additional-ro-crate-metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/moises/source/github/Language-Research-Technology/ro-crate-excel/test_data/additional/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DA679FC-E309-5140-B031-83412ADD97D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E5A905A-8F49-CF41-B4D3-50E5DE816EC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="People" sheetId="7" r:id="rId1"/>
@@ -2114,8 +2114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2184,8 +2184,8 @@
         <v>1</v>
       </c>
       <c r="G2" t="str">
-        <f>H2</f>
-        <v>#AUDIO_Rosa</v>
+        <f>Objects!A2</f>
+        <v>#OBJECT_Rosa</v>
       </c>
       <c r="H2" t="str">
         <f>_xlfn.CONCAT("#",C2)</f>
@@ -2221,11 +2221,11 @@
         <v>1</v>
       </c>
       <c r="G3" t="str">
-        <f t="shared" ref="G3:G5" si="2">H3</f>
-        <v>#AUDIO_Juan</v>
+        <f>Objects!A3</f>
+        <v>#OBJECT_Juan</v>
       </c>
       <c r="H3" t="str">
-        <f t="shared" ref="H3:H5" si="3">_xlfn.CONCAT("#",C3)</f>
+        <f t="shared" ref="H3:H5" si="2">_xlfn.CONCAT("#",C3)</f>
         <v>#AUDIO_Juan</v>
       </c>
       <c r="I3" t="str">
@@ -2258,11 +2258,11 @@
         <v>1</v>
       </c>
       <c r="G4" t="str">
+        <f>Objects!A4</f>
+        <v>#OBJECT_Emilia</v>
+      </c>
+      <c r="H4" t="str">
         <f t="shared" si="2"/>
-        <v>#AUDIO_Emilia</v>
-      </c>
-      <c r="H4" t="str">
-        <f t="shared" si="3"/>
         <v>#AUDIO_Emilia</v>
       </c>
       <c r="I4" t="str">
@@ -2295,11 +2295,11 @@
         <v>1</v>
       </c>
       <c r="G5" t="str">
+        <f>Objects!A5</f>
+        <v>#OBJECT_Maria</v>
+      </c>
+      <c r="H5" t="str">
         <f t="shared" si="2"/>
-        <v>#AUDIO_Maria</v>
-      </c>
-      <c r="H5" t="str">
-        <f t="shared" si="3"/>
         <v>#AUDIO_Maria</v>
       </c>
       <c r="I5" t="str">
@@ -2319,8 +2319,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2547,7 +2547,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>